<commit_message>
Updated f3ds und pcb export
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SM-Projekte\OSSM-M5-Remote\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8CD3EF3D-8BBB-46D1-A68D-04117E352D04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E02470B-C71B-47DB-ACB5-EA4BB5C73A77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{EF1F950B-B24B-4156-88EB-AFA567968960}"/>
+    <workbookView xWindow="28650" yWindow="-16410" windowWidth="29040" windowHeight="15720" xr2:uid="{EF1F950B-B24B-4156-88EB-AFA567968960}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -48,9 +48,6 @@
     <t>Stk</t>
   </si>
   <si>
-    <t>EK</t>
-  </si>
-  <si>
     <t>Price Per Part</t>
   </si>
   <si>
@@ -70,6 +67,9 @@
   </si>
   <si>
     <t>Female Pin Header 2x15 Pins 11mm (Unit)</t>
+  </si>
+  <si>
+    <t>Buy-Price</t>
   </si>
 </sst>
 </file>
@@ -455,7 +455,7 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -478,13 +478,13 @@
         <v>3</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" t="s">
         <v>4</v>
       </c>
-      <c r="E2" t="s">
+      <c r="G2" t="s">
         <v>5</v>
-      </c>
-      <c r="G2" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -511,7 +511,7 @@
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4">
         <v>1000</v>
@@ -520,7 +520,7 @@
         <v>9</v>
       </c>
       <c r="E4" s="2">
-        <f t="shared" ref="E4:E10" si="0">C4/B4</f>
+        <f t="shared" ref="E4:E8" si="0">C4/B4</f>
         <v>8.9999999999999993E-3</v>
       </c>
       <c r="G4">
@@ -533,7 +533,7 @@
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5">
         <v>10</v>
@@ -555,7 +555,7 @@
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B6">
         <v>20</v>
@@ -577,7 +577,7 @@
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B7">
         <v>20</v>
@@ -599,7 +599,7 @@
     </row>
     <row r="8" spans="1:8" ht="17.25">
       <c r="A8" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B8">
         <v>20</v>

</xml_diff>